<commit_message>
fixed bugs and now tuning eqs
</commit_message>
<xml_diff>
--- a/route_processed.xlsx
+++ b/route_processed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Op Seq</t>
   </si>
@@ -31,34 +31,10 @@
     <t>إنشاءات</t>
   </si>
   <si>
-    <t xml:space="preserve">الرمالة </t>
-  </si>
-  <si>
-    <t>دهان رش</t>
-  </si>
-  <si>
-    <t>لحام بنطة</t>
-  </si>
-  <si>
-    <t>لحام يدوي</t>
-  </si>
-  <si>
-    <t>تجليخ</t>
-  </si>
-  <si>
-    <t>ترميل</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ماكينة لحام </t>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
-    <t>رمالة</t>
-  </si>
-  <si>
-    <t>خـــط رش يـــدوي</t>
+    <t>قطع ليزر</t>
+  </si>
+  <si>
+    <t>ماكينة قطع باليزر 3 م</t>
   </si>
 </sst>
 </file>
@@ -416,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -447,78 +423,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
         <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stopped at drl equation
</commit_message>
<xml_diff>
--- a/route_processed.xlsx
+++ b/route_processed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Op Seq</t>
   </si>
@@ -28,13 +28,16 @@
     <t>machine</t>
   </si>
   <si>
-    <t>إنشاءات</t>
-  </si>
-  <si>
-    <t>قطع ليزر</t>
-  </si>
-  <si>
-    <t>ماكينة قطع باليزر 3 م</t>
+    <t>no of cuts</t>
+  </si>
+  <si>
+    <t>منطقة 2</t>
+  </si>
+  <si>
+    <t>ثقب</t>
+  </si>
+  <si>
+    <t>مثقاب</t>
   </si>
 </sst>
 </file>
@@ -392,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -411,8 +414,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -420,13 +426,16 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>